<commit_message>
Update comparison of PhUSE data synthesis projects
</commit_message>
<xml_diff>
--- a/PhUSE - Compare Synthetic Data Projects.xlsx
+++ b/PhUSE - Compare Synthetic Data Projects.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E0459231\dev\TestDataFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA1F1D5A-BC9F-4E69-B83C-D7BC342EACA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C886791-47E4-4C8A-B82A-06042644F765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13605" yWindow="-14760" windowWidth="21600" windowHeight="11505" xr2:uid="{0C12DAA8-0303-4EF6-9C44-BB376B97AA69}"/>
+    <workbookView xWindow="10245" yWindow="-15975" windowWidth="26685" windowHeight="15465" activeTab="1" xr2:uid="{0C12DAA8-0303-4EF6-9C44-BB376B97AA69}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId1"/>
+    <sheet name="Compare" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Project</t>
   </si>
@@ -84,9 +85,6 @@
   </si>
   <si>
     <t>Creating a program that runs with a GUI, allows selection of output domains, study type, and creates the full dataset. This program can be run either locally by a user, or eventually from a cloud based public location.</t>
-  </si>
-  <si>
-    <t>Running program, that creates most SEND domain output for basic tox study. Not yet checked with validator, not all fields generated. Uses for some domains known ranges of data for different species.</t>
   </si>
   <si>
     <t>Dante Di Tommaso</t>
@@ -140,10 +138,6 @@
     <t>Create credible, CDISC-conformant clinical databases</t>
   </si>
   <si>
-    <t>Front-end proof-of-concept (R), 
-Back-end databases &amp; APIs (python)</t>
-  </si>
-  <si>
     <t>SAS, R and Python. Partly redundancy (started in SAS and R, then back-end/db/API progressed in Python &amp; graph db)</t>
   </si>
   <si>
@@ -151,12 +145,6 @@
   </si>
   <si>
     <t>https://github.com/phuse-org/SEND-TestDataFactory</t>
-  </si>
-  <si>
-    <t>Use case 1: Create targetted clinical databases to test software and applications. Ability to configure anomalies for test purposes.</t>
-  </si>
-  <si>
-    <t>Use case 2: Create credible clinical databases based on protocol/analysis plans, in order to progress study activities in advance of live data</t>
   </si>
   <si>
     <t>• Create datasets as standards are approaching finalization for testing systems that receive data from the standard</t>
@@ -242,11 +230,6 @@
     </r>
   </si>
   <si>
-    <t>• Overall design
-• Atomic modules, such as simulating datetimes, normal reals, etc.
-• Credible-data approach</t>
-  </si>
-  <si>
     <t>• Time intervals, durations, etc
 • Numeric distributions, specific to controlled terms (e.g., test names)
 • Findings responding to administrations, to simulate dose response
@@ -256,6 +239,136 @@
 ===
 Full model on these characteristics not developed.
 Need to take into account lab abnormalities.</t>
+  </si>
+  <si>
+    <t>R Package - CDISC Synthesis</t>
+  </si>
+  <si>
+    <t>Conformance</t>
+  </si>
+  <si>
+    <t>Teams location:</t>
+  </si>
+  <si>
+    <t>https://github.com/phuse-org/TestDataFactory/blob/main/PhUSE%20-%20Compare%20Synthetic%20Data%20Projects.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use case 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create targetted clinical databases to test software and applications. Ability to configure anomalies for test purposes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use case 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create credible clinical databases based on protocol/analysis plans, in order to progress study activities in advance of live data</t>
+    </r>
+  </si>
+  <si>
+    <t>R package</t>
+  </si>
+  <si>
+    <t>• Overall design
+• Atomic modules, such as simulating datetimes, normal reals, etc.
+• Credible-data approach
+• Missing data patterns
+• Variable-dependency definitions</t>
+  </si>
+  <si>
+    <t>Synthesize database from configuration</t>
+  </si>
+  <si>
+    <t>• generic variable generating functions
+• ability to extend these functions
+• R script approach from generating function</t>
+  </si>
+  <si>
+    <t>Python code
+SAS / CSV datasets created</t>
+  </si>
+  <si>
+    <t>• Synthetic personal health records
+• 100% synthetic
+• 100% scientific, based on industry databases, including registered marketed products, FDA/EMA
+• Could stop excluding veterinary components</t>
+  </si>
+  <si>
+    <t>Running program, that creates most SEND domain output for basic tox study. Not yet checked with validator, not all fields generated. Uses for some domains known ranges of data for different species.
+• 16 of 28 domains implemented
+• Conformance remains in progress - validation errors</t>
+  </si>
+  <si>
+    <t>Front-end proof-of-concept (R), 
+Back-end databases &amp; APIs (python)
+• Trial Design domains
+• DM - 3 variable types (CT, datetime)
+• LB/VS - config concepts defined</t>
+  </si>
+  <si>
+    <t>• 13 ADaM data sets implemented</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use case 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Test and document software for standard reporting</t>
+    </r>
+  </si>
+  <si>
+    <t>including:
+https://www.pinnacle21.com/validation-rules/sdtm</t>
+  </si>
+  <si>
+    <t>including:
+https://www.pinnacle21.com/validation-rules/send</t>
+  </si>
+  <si>
+    <t>• CDISC / P21 - basics
+• Expertise - study-specific disease, intervention, findings experience &amp; intuition</t>
   </si>
 </sst>
 </file>
@@ -308,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,12 +434,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -335,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -353,6 +490,34 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -669,276 +834,363 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D25CA0-2777-4263-8348-9134ABA33535}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{65F2E4BC-9BDE-419D-A3A4-523E255C268B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BD2250-CD5E-4186-83A6-67EB870B2A50}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="4" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="60.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="60.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="5" t="s">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D19" r:id="rId1" xr:uid="{D6A9448B-22B0-4B59-A4A2-FAAB69BD980D}"/>
-    <hyperlink ref="E19" r:id="rId2" xr:uid="{7CDBDEBC-F2FC-4C68-B7A6-C7CCB9631208}"/>
+    <hyperlink ref="E20" r:id="rId1" xr:uid="{D6A9448B-22B0-4B59-A4A2-FAAB69BD980D}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{7CDBDEBC-F2FC-4C68-B7A6-C7CCB9631208}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>